<commit_message>
lil change on burger_flow
</commit_message>
<xml_diff>
--- a/Burger_Flow.xlsx
+++ b/Burger_Flow.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\ryu19\Assignment\funfunassignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73128A2-044E-44A1-8624-2859FE84A8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA831DF7-7F47-42A9-AA20-F218B531CE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17250" yWindow="2235" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{D0A791DF-7743-4BF4-B387-694C194087D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{D0A791DF-7743-4BF4-B387-694C194087D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -962,7 +962,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,7 +1677,7 @@
         <v>3</v>
       </c>
       <c r="M24" s="15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N24" s="15"/>
       <c r="O24" s="15"/>

</xml_diff>